<commit_message>
Update - Start Of Formatting
AUTOENCODER DONE
- Start autoencoder documention in next release
</commit_message>
<xml_diff>
--- a/Deep Learning/BRAIN MRI/processed/meta.xlsx
+++ b/Deep Learning/BRAIN MRI/processed/meta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mini Projects\ML\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Mini Projects\ML\experiment\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{374B266E-D879-4C1A-887A-F2EB0689E083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8836B8-2965-4F5E-93D5-BDC18AA268A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2730" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1068,42 +1068,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+      <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1446,541 +1429,541 @@
   <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="8" style="6" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="6.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="7.5" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="46" style="6" customWidth="1"/>
-    <col min="13" max="13" width="3.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.33203125" style="6"/>
+    <col min="1" max="1" width="22.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="46" style="3" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.33203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10">
+      <c r="B1" s="2">
         <v>54</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="C1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="2">
         <v>25</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="C2" s="2"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="2">
         <v>20</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
+      <c r="C3" s="2"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="2">
         <v>27</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="C4" s="2"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="2">
         <v>24</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="7"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="C5" s="2"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="2">
         <v>22</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="C6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="2">
         <v>36</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="C7" s="2"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="2">
         <v>33</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="C8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="2">
         <v>23</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="C9" s="2"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="2">
         <v>41</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="C10" s="2"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="2">
         <v>27</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="C11" s="2"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="2">
         <v>28</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="9" t="s">
+      <c r="C12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="2">
         <v>26</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="C13" s="2"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="2">
         <v>19</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="9" t="s">
+      <c r="C14" s="2"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="2">
         <v>29</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="9" t="s">
+      <c r="C15" s="2"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="2">
         <v>55</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="7"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="9" t="s">
+      <c r="C16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="2">
         <v>40</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+      <c r="C17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="2">
         <v>43</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+      <c r="C18" s="2"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="2">
         <v>28</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="C19" s="2"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="2">
         <v>26</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+      <c r="C20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="2">
         <v>26</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="7"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+      <c r="C21" s="2"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="2">
         <v>39</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="7"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
+      <c r="C22" s="2"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="2">
         <v>40</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="9" t="s">
+      <c r="C23" s="2"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="2">
         <v>57</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="9" t="s">
+      <c r="C24" s="2"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="2">
         <v>49</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
+      <c r="C25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="2">
         <v>26</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="7"/>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="C26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="2">
         <v>48</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+      <c r="C27" s="2"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="10">
+      <c r="B28" s="2">
         <v>66</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="7"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
+      <c r="C28" s="2"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="3">
         <v>72</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="2">
         <v>57</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+      <c r="C30" s="2"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="2">
         <v>50</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+      <c r="C31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="2">
         <v>66</v>
       </c>
-      <c r="C32" s="10"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="7"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+      <c r="C32" s="2"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="2">
         <v>23</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="C33" s="2"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="2">
         <v>23</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="7"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="C34" s="2"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1988,7 +1971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1996,7 +1979,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2004,7 +1987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2012,7 +1995,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2020,7 +2003,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2028,15 +2011,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2044,7 +2027,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2052,7 +2035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2060,7 +2043,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2068,7 +2051,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2076,7 +2059,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -2084,15 +2067,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="6">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -2100,7 +2083,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -2108,7 +2091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -2116,7 +2099,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -2124,7 +2107,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -2132,7 +2115,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -2140,7 +2123,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -2148,15 +2131,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
+    <row r="56" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B56" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -2164,7 +2147,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>55</v>
       </c>
@@ -2172,7 +2155,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>56</v>
       </c>
@@ -2180,7 +2163,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>57</v>
       </c>
@@ -2188,7 +2171,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>58</v>
       </c>
@@ -2196,7 +2179,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>59</v>
       </c>
@@ -2204,7 +2187,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>60</v>
       </c>
@@ -2212,7 +2195,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>61</v>
       </c>
@@ -2220,7 +2203,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>62</v>
       </c>
@@ -2228,7 +2211,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>63</v>
       </c>
@@ -2236,7 +2219,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>64</v>
       </c>
@@ -2244,7 +2227,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>65</v>
       </c>
@@ -2252,7 +2235,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>66</v>
       </c>
@@ -2260,7 +2243,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>67</v>
       </c>
@@ -2268,7 +2251,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>68</v>
       </c>
@@ -2276,7 +2259,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>69</v>
       </c>
@@ -2284,7 +2267,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>70</v>
       </c>
@@ -2292,7 +2275,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>71</v>
       </c>
@@ -2300,7 +2283,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>72</v>
       </c>
@@ -2308,7 +2291,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>73</v>
       </c>
@@ -2316,7 +2299,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>74</v>
       </c>
@@ -2324,7 +2307,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>75</v>
       </c>
@@ -2332,7 +2315,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>76</v>
       </c>
@@ -2340,7 +2323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
@@ -2348,7 +2331,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2356,7 +2339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>79</v>
       </c>
@@ -2364,7 +2347,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>80</v>
       </c>
@@ -2372,15 +2355,15 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="6">
         <v>67</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -2388,7 +2371,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>83</v>
       </c>
@@ -2396,7 +2379,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>84</v>
       </c>
@@ -2404,7 +2387,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -2412,7 +2395,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>86</v>
       </c>
@@ -2420,7 +2403,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -2428,15 +2411,15 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
+    <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B91" s="4">
+      <c r="B91" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>89</v>
       </c>
@@ -2444,7 +2427,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>90</v>
       </c>
@@ -2452,7 +2435,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>91</v>
       </c>
@@ -2460,7 +2443,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>92</v>
       </c>
@@ -2468,7 +2451,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>93</v>
       </c>
@@ -2476,7 +2459,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>94</v>
       </c>
@@ -2484,15 +2467,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="5">
+      <c r="B98" s="6">
         <v>64</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>96</v>
       </c>

</xml_diff>